<commit_message>
"Erweiterung der Eingabe- und Exportfunktionen, Hinzufügen von neuen Parametern zu `Kurschlusskräfte_Input`, Anpassung der Berechnungslogik, Verbesserung der GUI mit zusätzlicher Eingabeverarbeitung und Download-Optionen sowie Optimierungen der Excel-Exportfunktion."
</commit_message>
<xml_diff>
--- a/data/Eingaben Vorlage.xlsx
+++ b/data/Eingaben Vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1d3018db502cb77/Documents/GitHub/Kurzschlussfestigkeit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{8F7288E3-DEE1-4B07-ACF4-8482EF9DFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7AB6A3B-2013-44E3-B389-31567E707ACC}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{8F7288E3-DEE1-4B07-ACF4-8482EF9DFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7069FDCF-2F3E-4DC5-B80B-2219C4639F08}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Quellen &amp; Versionen" sheetId="19" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -206,13 +207,13 @@
     <numFmt numFmtId="167" formatCode="&quot;CHF&quot;* #,##0.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.0\ &quot;MVA&quot;"/>
     <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;m&quot;"/>
-    <numFmt numFmtId="175" formatCode="#,##0.0"/>
-    <numFmt numFmtId="177" formatCode="##0\ &quot;°C&quot;"/>
-    <numFmt numFmtId="178" formatCode="#,##0.0\ &quot;kA&quot;"/>
-    <numFmt numFmtId="179" formatCode="#,##0.0\ &quot;s&quot;"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00\ &quot;kg&quot;"/>
-    <numFmt numFmtId="183" formatCode="#,##0.00\ &quot;kN&quot;"/>
-    <numFmt numFmtId="184" formatCode="#,##0\ &quot;N/m&quot;"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0"/>
+    <numFmt numFmtId="171" formatCode="##0\ &quot;°C&quot;"/>
+    <numFmt numFmtId="172" formatCode="#,##0.0\ &quot;kA&quot;"/>
+    <numFmt numFmtId="173" formatCode="#,##0.0\ &quot;s&quot;"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;kg&quot;"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00\ &quot;kN&quot;"/>
+    <numFmt numFmtId="176" formatCode="#,##0\ &quot;N/m&quot;"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -931,7 +932,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="22" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1001,116 +1002,41 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="20" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="175" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1119,6 +1045,78 @@
     <xf numFmtId="49" fontId="20" fillId="33" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="8" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1183,6 +1181,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1420,19 +1422,19 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1441,7 +1443,7 @@
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="37" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="1"/>
@@ -1453,7 +1455,7 @@
       <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="38" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="1"/>
@@ -1465,7 +1467,7 @@
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="38" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="1"/>
@@ -1477,7 +1479,7 @@
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="1"/>
@@ -1489,7 +1491,7 @@
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="30">
         <v>-20</v>
       </c>
     </row>
@@ -1497,21 +1499,21 @@
       <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="31">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="48"/>
+      <c r="B11" s="40"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="32">
         <v>40</v>
       </c>
     </row>
@@ -1519,7 +1521,7 @@
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="53">
+      <c r="B13" s="28">
         <v>1.8</v>
       </c>
     </row>
@@ -1527,21 +1529,21 @@
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="58">
+      <c r="B14" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="48"/>
+      <c r="B15" s="40"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="37" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1549,7 +1551,7 @@
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="54">
+      <c r="B17" s="29">
         <v>2</v>
       </c>
     </row>
@@ -1557,21 +1559,21 @@
       <c r="A18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="59">
+      <c r="B18" s="34">
         <v>15.3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="48"/>
+      <c r="B19" s="40"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="25">
         <v>25</v>
       </c>
     </row>
@@ -1579,7 +1581,7 @@
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="25">
         <v>1.5</v>
       </c>
     </row>
@@ -1587,7 +1589,7 @@
       <c r="A22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="25">
         <v>2</v>
       </c>
     </row>
@@ -1595,21 +1597,21 @@
       <c r="A23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="25">
         <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="48"/>
+      <c r="B24" s="40"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="60">
+      <c r="B25" s="35">
         <v>15.5</v>
       </c>
     </row>
@@ -1617,29 +1619,29 @@
       <c r="A26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="60">
+      <c r="B26" s="35">
         <v>12.5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="61">
+      <c r="B27" s="36">
         <v>100000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="48"/>
+      <c r="B28" s="40"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="49">
+      <c r="B29" s="25">
         <v>5</v>
       </c>
     </row>
@@ -1647,15 +1649,15 @@
       <c r="A30" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="49">
+      <c r="B30" s="25">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="49">
+      <c r="B31" s="25">
         <v>15</v>
       </c>
     </row>
@@ -1663,45 +1665,45 @@
       <c r="A32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="49">
+      <c r="B32" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="49"/>
+      <c r="B33" s="25"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="49"/>
+      <c r="B34" s="25"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="50" t="s">
+      <c r="A35" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="49"/>
+      <c r="B35" s="25"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="49"/>
+      <c r="B36" s="25"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="49"/>
+      <c r="B37" s="25"/>
     </row>
     <row r="38" spans="1:2" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="52"/>
+      <c r="B38" s="27"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
@@ -1887,14 +1889,7 @@
       <formula1>"100000, 150000, 1300000, 400000, 2000000, 600000, 3000000"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{DD76BAA2-9D59-4DB8-852A-41AA0F911BDB}">
-      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="x12ac">
-          <x12ac:list>16-AL1 (16), 24-AL1 (25), 34-AL1 (35), 49-AL1 (50), 48-AL1 (50), 66-AL1 (70), 93-AL1 (95), 117-AL1 (120), 147-AL1 (150), 182-AL1 (185), 243-AL1 (240), 299-AL1 (300), 400-AL1 (400), 500-AL1 (500), 626-AL1 (625), 802-AL1 (800), 1000-AL1 (1000), 16-AL3 (16), 24-AL3 (25), 34-AL3 (35), 49-AL3 (50), 66-AL3 (70), 93-AL3 (95), 117-AL3 (120), 147-AL3 (150), 182-AL3 (185), 243-AL3 (240), 299-AL3 (300), 400-AL3 (400), 500-AL3 (500), 626-AL3 (625), 802-AL3 (800), 1000-AL3 (1000), 22-AL4 (ASTER 22)," 34-AL4 (ASTER 34,4)"," 55-AL4 (ASTER 54,6)"," 76-AL4 (ASTER 75,5)", 117-AL4 (ASTER 117), 148-AL4 (ASTER 148)," 182-AL4 (ASTER 181,6)", 228-AL4 (ASTER 228), 228-AL4 (ASTER 288), 366-AL4 (ASTER 366), 570-AL4 (ASTER 570), 851-AL4 (ASTER 851), 1144-AL4 (ASTER 1144)," 1600-AL4 (1596-AL4, ASTER 1600)"," 15-AL1/3-ST1A (16/2,5)", 24-AL1/4-ST1A (25/4), 34-AL1/6-ST1A (35/6), 44-AL1/32-ST1A (44/32), 48-AL1/8-ST1A (50/8), 51-AL1/30-ST1A (50/30), 70-AL1/11-ST1A (70/12), 94-AL1/15-ST1A (95/15), 97-AL1/56-ST1A (95/55), 106-AL1/76-ST1A (105/75), 122-AL1/20-ST1A (120/20), 122-AL1/71-ST1A (120/70), 128-AL1/30-ST1A (125/30), 149-AL1/24-ST1A (150/25), 172-AL1/40-ST1A (170/40), 184-AL1/30-ST1A (185/30), 209-AL1/34-ST1A (210/35), 212-AL1/49-ST1A (210/50), 231-AL1/30-ST1A (230/30), 243-AL1/39-ST1A (240/40), 264-AL1/34-ST1A (265/35), 304-AL1/49-ST1A (300/50), 305-AL1/39-ST1A (305/40), 339-AL1/30-ST1A (340/30), 382-AL1/49-ST1A (380/50), 386-AL1/34-ST1A (385/35), 434-AL1/56-ST1A (435/55), 449-AL1/39-ST1A (450/40), 490-AL1/64-ST1A (490/65), 494-AL1/34-ST1A (495/35), 511-AL1/45-ST1A (510/45), 550-AL1/71-ST1A (550/70), 562-AL1/49-ST1A (560/50), 571-AL1/39-ST1A (570/40), 653-AL1/45-ST1A (650/45), 679-AL1/86-ST1A (680/85), 1046-AL1/45-ST1A (1045/45)," 15-AL3/3-ST1A (16/2,5)", 24-AL3/ 4-ST1A (25/4), 34-AL3/ 6-ST1A (35/6), 44-AL3/32-ST1A (44/32), 48-AL3/ 8-ST1A (50/8), 51-AL3/30-ST1A (50/30), 70-AL3/ 11-ST1A (70/12), 94-AL3/ 22-ST1A (94/22), 94-AL3/ 15-ST1A (95/15), 97-AL3/ 34-ST1A (95/55), 106-AL3/76-ST1A (105/75), 122-AL3/ 20-ST1A (120/20), 122-AL3/ 71-ST1A (120/70), 128-AL3/ 30-ST1A (125/30), 149-AL3/ 24-ST1A (150/25), 172-AL3/ 40-ST1A (170/40), 184-AL3/ 30-ST1A (185/30), 209-AL3/ 34-ST1A (210/35), 212-AL3/ 49-ST1A (210/50), 231-AL3/ 30-ST1A (230/30), 243-AL3/ 39-ST1A (240/40), 264-AL3/ 34-ST1A (265/35), 304-AL3/ 49-ST1A (300/50), 305-AL3/ 39-ST1A (305/40), 339-AL3/ 30-ST1A (340/30), 382-AL3/ 49-ST1A (380/50), 386-AL3/ 34-ST1A (385/35), 434-AL3/ 56-ST1A (435/55), 449-AL3/ 39-ST1A (450/40), 490-AL3/ 64-ST1A (490/65), 550-AL3/ 71-ST1A (550/70), 562-AL3/ 49-ST1A (560/50), 679-AL3/ 86-ST1A (680/85), 24-A20SA (25), 34-A20SA (35), 49-A20SA (50), 66-A20SA (70), 93-A20SA (95), 117-A20SA (120), 147-A20SA (150), 182-A20SA (185), 243-A20SA (240), 299-A20SA (300), DIN 48201-500-E-Cu, DIN 48201-400-E-Cu, DIN 48201-300-E-Cu, DIN 48201-240-E-Cu, DIN 48201-185-E-Cu, DIN 48201-150-E-Cu, DIN 48201-120-E-Cu, DIN 48201-95-E-Cu, DIN 48201-70-E-Cu, DIN 48201-50/19-E-Cu, DIN 48201-50/7-E-Cu, DIN 48201-35-E-Cu, DIN 48201-25-E-Cu, DIN 48201-16-E-Cu, DIN 48201-10-E-Cu, Bronze-Seil 10, Bronze-Seil 16, Bronze-Seil 25, Bronze-Seil 35, Bronze-Seil 50, Bronze-Seil 50, Bronze-Seil 70, Bronze-Seil 95, Bronze-Seil 120, Bronze-Seil 150, Bronze-Seil 185, Bronze-Seil 240, Bronze-Seil 300, Bronze-Seil 400, Bronze-Seil 500</x12ac:list>
-        </mc:Choice>
-        <mc:Fallback>
-          <formula1>_xlfn._LONGTEXT("16-AL1 (16), 24-AL1 (25), 34-AL1 (35), 49-AL1 (50), 48-AL1 (50), 66-AL1 (70), 93-AL1 (95), 117-AL1 (120), 147-AL1 (150), 182-AL1 (185), 243-AL1 (240), 299-AL1 (300), 400-AL1 (400), 500-AL1 (500), 626-AL1 (625), 802-AL1 (800), 1000-AL1 (1000), 16-AL3 (16),"," 24-AL3 (25), 34-AL3 (35), 49-AL3 (50), 66-AL3 (70), 93-AL3 (95), 117-AL3 (120), 147-AL3 (150), 182-AL3 (185), 243-AL3 (240), 299-AL3 (300), 400-AL3 (400), 500-AL3 (500), 626-AL3 (625), 802-AL3 (800), 1000-AL3 (1000), 22-AL4 (ASTER 22), 34-AL4 (ASTER 34,4","), 55-AL4 (ASTER 54,6), 76-AL4 (ASTER 75,5), 117-AL4 (ASTER 117), 148-AL4 (ASTER 148), 182-AL4 (ASTER 181,6), 228-AL4 (ASTER 228), 228-AL4 (ASTER 288), 366-AL4 (ASTER 366), 570-AL4 (ASTER 570), 851-AL4 (ASTER 851), 1144-AL4 (ASTER 1144), 1600-AL4 (1596-AL","4, ASTER 1600), 15-AL1/3-ST1A (16/2,5), 24-AL1/4-ST1A (25/4), 34-AL1/6-ST1A (35/6), 44-AL1/32-ST1A (44/32), 48-AL1/8-ST1A (50/8), 51-AL1/30-ST1A (50/30), 70-AL1/11-ST1A (70/12), 94-AL1/15-ST1A (95/15), 97-AL1/56-ST1A (95/55), 106-AL1/76-ST1A (105/75), 122","-AL1/20-ST1A (120/20), 122-AL1/71-ST1A (120/70), 128-AL1/30-ST1A (125/30), 149-AL1/24-ST1A (150/25), 172-AL1/40-ST1A (170/40), 184-AL1/30-ST1A (185/30), 209-AL1/34-ST1A (210/35), 212-AL1/49-ST1A (210/50), 231-AL1/30-ST1A (230/30), 243-AL1/39-ST1A (240/40)",", 264-AL1/34-ST1A (265/35), 304-AL1/49-ST1A (300/50), 305-AL1/39-ST1A (305/40), 339-AL1/30-ST1A (340/30), 382-AL1/49-ST1A (380/50), 386-AL1/34-ST1A (385/35), 434-AL1/56-ST1A (435/55), 449-AL1/39-ST1A (450/40), 490-AL1/64-ST1A (490/65), 494-AL1/34-ST1A (49","5/35), 511-AL1/45-ST1A (510/45), 550-AL1/71-ST1A (550/70), 562-AL1/49-ST1A (560/50), 571-AL1/39-ST1A (570/40), 653-AL1/45-ST1A (650/45), 679-AL1/86-ST1A (680/85), 1046-AL1/45-ST1A (1045/45), 15-AL3/3-ST1A (16/2,5), 24-AL3/ 4-ST1A (25/4), 34-AL3/ 6-ST1A (3","5/6), 44-AL3/32-ST1A (44/32), 48-AL3/ 8-ST1A (50/8), 51-AL3/30-ST1A (50/30), 70-AL3/ 11-ST1A (70/12), 94-AL3/ 22-ST1A (94/22), 94-AL3/ 15-ST1A (95/15), 97-AL3/ 34-ST1A (95/55), 106-AL3/76-ST1A (105/75), 122-AL3/ 20-ST1A (120/20), 122-AL3/ 71-ST1A (120/70)",", 128-AL3/ 30-ST1A (125/30), 149-AL3/ 24-ST1A (150/25), 172-AL3/ 40-ST1A (170/40), 184-AL3/ 30-ST1A (185/30), 209-AL3/ 34-ST1A (210/35), 212-AL3/ 49-ST1A (210/50), 231-AL3/ 30-ST1A (230/30), 243-AL3/ 39-ST1A (240/40), 264-AL3/ 34-ST1A (265/35), 304-AL3/ 4","9-ST1A (300/50), 305-AL3/ 39-ST1A (305/40), 339-AL3/ 30-ST1A (340/30), 382-AL3/ 49-ST1A (380/50), 386-AL3/ 34-ST1A (385/35), 434-AL3/ 56-ST1A (435/55), 449-AL3/ 39-ST1A (450/40), 490-AL3/ 64-ST1A (490/65), 550-AL3/ 71-ST1A (550/70), 562-AL3/ 49-ST1A (560/","50), 679-AL3/ 86-ST1A (680/85), 24-A20SA (25), 34-A20SA (35), 49-A20SA (50), 66-A20SA (70), 93-A20SA (95), 117-A20SA (120), 147-A20SA (150), 182-A20SA (185), 243-A20SA (240), 299-A20SA (300), DIN 48201-500-E-Cu, DIN 48201-400-E-Cu, DIN 48201-300-E-Cu, DIN"," 48201-240-E-Cu, DIN 48201-185-E-Cu, DIN 48201-150-E-Cu, DIN 48201-120-E-Cu, DIN 48201-95-E-Cu, DIN 48201-70-E-Cu, DIN 48201-50/19-E-Cu, DIN 48201-50/7-E-Cu, DIN 48201-35-E-Cu, DIN 48201-25-E-Cu, DIN 48201-16-E-Cu, DIN 48201-10-E-Cu, Bronze-Seil 10, Bronz","e-Seil 16, Bronze-Seil 25, Bronze-Seil 35, Bronze-Seil 50, Bronze-Seil 50, Bronze-Seil 70, Bronze-Seil 95, Bronze-Seil 120, Bronze-Seil 150, Bronze-Seil 185, Bronze-Seil 240, Bronze-Seil 300, Bronze-Seil 400, Bronze-Seil 500")</formula1>
-        </mc:Fallback>
-      </mc:AlternateContent>
+      <formula1>_xlfn._LONGTEXT("16-AL1 (16); 24-AL1 (25); 34-AL1 (35); 49-AL1 (50); 48-AL1 (50); 66-AL1 (70); 93-AL1 (95); 117-AL1 (120); 147-AL1 (150); 182-AL1 (185); 243-AL1 (240); 299-AL1 (300); 400-AL1 (400); 500-AL1 (500); 626-AL1 (625); 802-AL1 (800); 1000-AL1 (1000); 16-AL3 (16);"," 24-AL3 (25); 34-AL3 (35); 49-AL3 (50); 66-AL3 (70); 93-AL3 (95); 117-AL3 (120); 147-AL3 (150); 182-AL3 (185); 243-AL3 (240); 299-AL3 (300); 400-AL3 (400); 500-AL3 (500); 626-AL3 (625); 802-AL3 (800); 1000-AL3 (1000); 22-AL4 (ASTER 22); 34-AL4 (ASTER 34,4","); 55-AL4 (ASTER 54,6); 76-AL4 (ASTER 75,5); 117-AL4 (ASTER 117); 148-AL4 (ASTER 148); 182-AL4 (ASTER 181,6); 228-AL4 (ASTER 228); 228-AL4 (ASTER 288); 366-AL4 (ASTER 366); 570-AL4 (ASTER 570); 851-AL4 (ASTER 851); 1144-AL4 (ASTER 1144); 1600-AL4 (1596-AL","4, ASTER 1600); 15-AL1/3-ST1A (16/2,5); 24-AL1/4-ST1A (25/4); 34-AL1/6-ST1A (35/6); 44-AL1/32-ST1A (44/32); 48-AL1/8-ST1A (50/8); 51-AL1/30-ST1A (50/30); 70-AL1/11-ST1A (70/12); 94-AL1/15-ST1A (95/15); 97-AL1/56-ST1A (95/55); 106-AL1/76-ST1A (105/75); 122","-AL1/20-ST1A (120/20); 122-AL1/71-ST1A (120/70); 128-AL1/30-ST1A (125/30); 149-AL1/24-ST1A (150/25); 172-AL1/40-ST1A (170/40); 184-AL1/30-ST1A (185/30); 209-AL1/34-ST1A (210/35); 212-AL1/49-ST1A (210/50); 231-AL1/30-ST1A (230/30); 243-AL1/39-ST1A (240/40)","; 264-AL1/34-ST1A (265/35); 304-AL1/49-ST1A (300/50); 305-AL1/39-ST1A (305/40); 339-AL1/30-ST1A (340/30); 382-AL1/49-ST1A (380/50); 386-AL1/34-ST1A (385/35); 434-AL1/56-ST1A (435/55); 449-AL1/39-ST1A (450/40); 490-AL1/64-ST1A (490/65); 494-AL1/34-ST1A (49","5/35); 511-AL1/45-ST1A (510/45); 550-AL1/71-ST1A (550/70); 562-AL1/49-ST1A (560/50); 571-AL1/39-ST1A (570/40); 653-AL1/45-ST1A (650/45); 679-AL1/86-ST1A (680/85); 1046-AL1/45-ST1A (1045/45); 15-AL3/3-ST1A (16/2,5); 24-AL3/ 4-ST1A (25/4); 34-AL3/ 6-ST1A (3","5/6); 44-AL3/32-ST1A (44/32); 48-AL3/ 8-ST1A (50/8); 51-AL3/30-ST1A (50/30); 70-AL3/ 11-ST1A (70/12); 94-AL3/ 22-ST1A (94/22); 94-AL3/ 15-ST1A (95/15); 97-AL3/ 34-ST1A (95/55); 106-AL3/76-ST1A (105/75); 122-AL3/ 20-ST1A (120/20); 122-AL3/ 71-ST1A (120/70)","; 128-AL3/ 30-ST1A (125/30); 149-AL3/ 24-ST1A (150/25); 172-AL3/ 40-ST1A (170/40); 184-AL3/ 30-ST1A (185/30); 209-AL3/ 34-ST1A (210/35); 212-AL3/ 49-ST1A (210/50); 231-AL3/ 30-ST1A (230/30); 243-AL3/ 39-ST1A (240/40); 264-AL3/ 34-ST1A (265/35); 304-AL3/ 4","9-ST1A (300/50); 305-AL3/ 39-ST1A (305/40); 339-AL3/ 30-ST1A (340/30); 382-AL3/ 49-ST1A (380/50); 386-AL3/ 34-ST1A (385/35); 434-AL3/ 56-ST1A (435/55); 449-AL3/ 39-ST1A (450/40); 490-AL3/ 64-ST1A (490/65); 550-AL3/ 71-ST1A (550/70); 562-AL3/ 49-ST1A (560/","50); 679-AL3/ 86-ST1A (680/85); 24-A20SA (25); 34-A20SA (35); 49-A20SA (50); 66-A20SA (70); 93-A20SA (95); 117-A20SA (120); 147-A20SA (150); 182-A20SA (185); 243-A20SA (240); 299-A20SA (300); DIN 48201-500-E-Cu; DIN 48201-400-E-Cu; DIN 48201-300-E-Cu; DIN"," 48201-240-E-Cu; DIN 48201-185-E-Cu; DIN 48201-150-E-Cu; DIN 48201-120-E-Cu; DIN 48201-95-E-Cu; DIN 48201-70-E-Cu; DIN 48201-50/19-E-Cu; DIN 48201-50/7-E-Cu; DIN 48201-35-E-Cu; DIN 48201-25-E-Cu; DIN 48201-16-E-Cu; DIN 48201-10-E-Cu; Bronze-Seil 10; Bronz","e-Seil 16; Bronze-Seil 25; Bronze-Seil 35; Bronze-Seil 50; Bronze-Seil 50; Bronze-Seil 70; Bronze-Seil 95; Bronze-Seil 120; Bronze-Seil 150; Bronze-Seil 185; Bronze-Seil 240; Bronze-Seil 300; Bronze-Seil 400; Bronze-Seil 500")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.55118110236220474" top="1.1811023622047245" bottom="0.78740157480314965" header="0.47244094488188981" footer="0.35433070866141736"/>
@@ -1937,10 +1932,10 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
@@ -1955,10 +1950,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
@@ -1973,186 +1968,186 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="19"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="19"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="46"/>
       <c r="C23" s="16"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="34"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="44"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="22"/>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -2161,15 +2156,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="L3JGn++vkSXlWLsCCYWWINtqUqmHh3ss+Y3UnfzvYnEO110ZTLt4h5Wk1J0P8sdh9gATNb+6gDKHOpRAIsir+Q==" saltValue="aQCLb7ecvUo3cSUIR9a0KA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="25">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
@@ -2186,6 +2172,15 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.55118110236220474" top="1.1811023622047245" bottom="0.9055118110236221" header="0.47244094488188981" footer="0.35433070866141736"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
@@ -2201,20 +2196,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="adda6a32-00d2-4666-b9cc-96528deec2dc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="adda6a32-00d2-4666-b9cc-96528deec2dc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2457,14 +2452,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ED21654-8749-4BDD-B9EA-E0D53BBAF9EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F9A37C5-3D7A-4DD3-B23A-F45CB37B838D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2477,6 +2464,14 @@
     <ds:schemaRef ds:uri="b3a9547a-1fca-4aa3-b835-aaa4e5970e64"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ED21654-8749-4BDD-B9EA-E0D53BBAF9EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>